<commit_message>
Add producer-comsumer data and plotter
Also include spreadsheets of previous data.
</commit_message>
<xml_diff>
--- a/data/indexer_data.xlsx
+++ b/data/indexer_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\q2qroject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\q2qroject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="684" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="684"/>
   </bookViews>
   <sheets>
     <sheet name="Indexer Transitions" sheetId="1" r:id="rId1"/>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,11 +686,6 @@
         <v>40102</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -701,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
First draft of SPOR section
</commit_message>
<xml_diff>
--- a/data/indexer_data.xlsx
+++ b/data/indexer_data.xlsx
@@ -393,7 +393,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>